<commit_message>
fix: Finaliza correções de lógica e dados
</commit_message>
<xml_diff>
--- a/src/main/resources/Templates/Informacoes_Empresas.xlsx
+++ b/src/main/resources/Templates/Informacoes_Empresas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MENICIO JR\Desktop\Natural2SPARQL-master\src\main\resources\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MENICIO JR\Desktop\Natural2SPARQL_2025\src\main\resources\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1E797B-3004-467E-B1F2-97728F99ED5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD50BB1A-9B20-4551-BFC3-6C6DFAD79351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2922,11 +2922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:F401"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2958,7 +2957,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2979,7 +2978,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -3000,7 +2999,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -3021,7 +3020,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -3084,7 +3083,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -3105,7 +3104,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -3126,7 +3125,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -3147,7 +3146,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -3168,7 +3167,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -3189,7 +3188,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -3210,7 +3209,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>812</v>
       </c>
@@ -3294,7 +3293,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>55</v>
       </c>
@@ -3315,7 +3314,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>57</v>
       </c>
@@ -3336,7 +3335,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>839</v>
       </c>
@@ -3357,7 +3356,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>62</v>
       </c>
@@ -3378,7 +3377,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>813</v>
       </c>
@@ -3399,7 +3398,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>67</v>
       </c>
@@ -3420,7 +3419,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>814</v>
       </c>
@@ -3441,7 +3440,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>70</v>
       </c>
@@ -3462,7 +3461,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>840</v>
       </c>
@@ -3483,7 +3482,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>815</v>
       </c>
@@ -3525,7 +3524,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>78</v>
       </c>
@@ -3546,7 +3545,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>82</v>
       </c>
@@ -3567,7 +3566,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>82</v>
       </c>
@@ -3588,7 +3587,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>87</v>
       </c>
@@ -3609,7 +3608,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>841</v>
       </c>
@@ -3630,7 +3629,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>816</v>
       </c>
@@ -3651,7 +3650,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>94</v>
       </c>
@@ -3672,7 +3671,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>94</v>
       </c>
@@ -3693,7 +3692,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>98</v>
       </c>
@@ -3714,7 +3713,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>837</v>
       </c>
@@ -3735,7 +3734,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>101</v>
       </c>
@@ -3756,7 +3755,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>101</v>
       </c>
@@ -3777,7 +3776,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>104</v>
       </c>
@@ -3798,7 +3797,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>108</v>
       </c>
@@ -3819,7 +3818,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>108</v>
       </c>
@@ -3840,7 +3839,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>111</v>
       </c>
@@ -3861,7 +3860,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>115</v>
       </c>
@@ -3882,7 +3881,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>115</v>
       </c>
@@ -3903,7 +3902,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>118</v>
       </c>
@@ -3924,7 +3923,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>120</v>
       </c>
@@ -3945,7 +3944,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>123</v>
       </c>
@@ -3966,7 +3965,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>125</v>
       </c>
@@ -3987,7 +3986,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>125</v>
       </c>
@@ -4008,7 +4007,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>128</v>
       </c>
@@ -4029,7 +4028,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>130</v>
       </c>
@@ -4050,7 +4049,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>132</v>
       </c>
@@ -4071,7 +4070,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>136</v>
       </c>
@@ -4092,7 +4091,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>817</v>
       </c>
@@ -4113,7 +4112,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>141</v>
       </c>
@@ -4134,7 +4133,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>145</v>
       </c>
@@ -4155,7 +4154,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>145</v>
       </c>
@@ -4176,7 +4175,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>145</v>
       </c>
@@ -4197,7 +4196,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>149</v>
       </c>
@@ -4218,7 +4217,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>151</v>
       </c>
@@ -4239,7 +4238,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>151</v>
       </c>
@@ -4260,7 +4259,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>157</v>
       </c>
@@ -4281,7 +4280,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>159</v>
       </c>
@@ -4302,7 +4301,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>818</v>
       </c>
@@ -4323,7 +4322,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>819</v>
       </c>
@@ -4344,7 +4343,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>820</v>
       </c>
@@ -4365,7 +4364,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>820</v>
       </c>
@@ -4386,7 +4385,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>165</v>
       </c>
@@ -4407,7 +4406,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>165</v>
       </c>
@@ -4428,7 +4427,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>821</v>
       </c>
@@ -4449,7 +4448,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>171</v>
       </c>
@@ -4470,7 +4469,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>171</v>
       </c>
@@ -4491,7 +4490,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>171</v>
       </c>
@@ -4512,7 +4511,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>175</v>
       </c>
@@ -4533,7 +4532,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>175</v>
       </c>
@@ -4554,7 +4553,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>178</v>
       </c>
@@ -4575,7 +4574,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>180</v>
       </c>
@@ -4596,7 +4595,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>183</v>
       </c>
@@ -4617,7 +4616,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>185</v>
       </c>
@@ -4659,7 +4658,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>822</v>
       </c>
@@ -4680,7 +4679,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>190</v>
       </c>
@@ -4764,7 +4763,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>196</v>
       </c>
@@ -4785,7 +4784,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>196</v>
       </c>
@@ -4827,7 +4826,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>202</v>
       </c>
@@ -4848,7 +4847,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>205</v>
       </c>
@@ -4869,7 +4868,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>205</v>
       </c>
@@ -4890,7 +4889,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>810</v>
       </c>
@@ -4911,7 +4910,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>804</v>
       </c>
@@ -5016,7 +5015,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>216</v>
       </c>
@@ -5058,7 +5057,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>220</v>
       </c>
@@ -5163,7 +5162,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>228</v>
       </c>
@@ -5184,7 +5183,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>823</v>
       </c>
@@ -5205,7 +5204,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>823</v>
       </c>
@@ -5226,7 +5225,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>232</v>
       </c>
@@ -5247,7 +5246,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>232</v>
       </c>
@@ -5268,7 +5267,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>824</v>
       </c>
@@ -5289,7 +5288,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>237</v>
       </c>
@@ -5310,7 +5309,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>241</v>
       </c>
@@ -5331,7 +5330,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>243</v>
       </c>
@@ -5352,7 +5351,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>245</v>
       </c>
@@ -5394,7 +5393,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>250</v>
       </c>
@@ -5415,7 +5414,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>252</v>
       </c>
@@ -5436,7 +5435,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>806</v>
       </c>
@@ -5457,7 +5456,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>806</v>
       </c>
@@ -5478,7 +5477,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>256</v>
       </c>
@@ -5499,7 +5498,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>256</v>
       </c>
@@ -5520,7 +5519,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>259</v>
       </c>
@@ -5541,7 +5540,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>261</v>
       </c>
@@ -5562,7 +5561,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>264</v>
       </c>
@@ -5583,7 +5582,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>266</v>
       </c>
@@ -5604,7 +5603,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>268</v>
       </c>
@@ -5625,7 +5624,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="129" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>270</v>
       </c>
@@ -5646,7 +5645,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="130" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>274</v>
       </c>
@@ -5667,7 +5666,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="131" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>274</v>
       </c>
@@ -5688,7 +5687,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="132" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>277</v>
       </c>
@@ -5709,7 +5708,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="133" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>279</v>
       </c>
@@ -5730,7 +5729,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="134" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>281</v>
       </c>
@@ -5751,7 +5750,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="135" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>283</v>
       </c>
@@ -5772,7 +5771,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>286</v>
       </c>
@@ -5793,7 +5792,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="137" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>290</v>
       </c>
@@ -5814,7 +5813,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>292</v>
       </c>
@@ -5940,7 +5939,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="144" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>303</v>
       </c>
@@ -5982,7 +5981,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="146" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>309</v>
       </c>
@@ -6003,7 +6002,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="147" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>805</v>
       </c>
@@ -6129,7 +6128,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>321</v>
       </c>
@@ -6150,7 +6149,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>323</v>
       </c>
@@ -6234,7 +6233,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="158" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>331</v>
       </c>
@@ -6255,7 +6254,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="159" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>333</v>
       </c>
@@ -6276,7 +6275,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="160" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>333</v>
       </c>
@@ -6297,7 +6296,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="161" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>337</v>
       </c>
@@ -6318,7 +6317,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="162" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>340</v>
       </c>
@@ -6339,7 +6338,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>340</v>
       </c>
@@ -6360,7 +6359,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="164" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>343</v>
       </c>
@@ -6381,7 +6380,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="165" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>345</v>
       </c>
@@ -6402,7 +6401,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>347</v>
       </c>
@@ -6423,7 +6422,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>349</v>
       </c>
@@ -6444,7 +6443,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>352</v>
       </c>
@@ -6465,7 +6464,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>354</v>
       </c>
@@ -6486,7 +6485,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>356</v>
       </c>
@@ -6507,7 +6506,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>825</v>
       </c>
@@ -6570,7 +6569,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="174" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>363</v>
       </c>
@@ -6591,7 +6590,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="175" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>365</v>
       </c>
@@ -6612,7 +6611,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>365</v>
       </c>
@@ -6633,7 +6632,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>368</v>
       </c>
@@ -6654,7 +6653,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>370</v>
       </c>
@@ -6675,7 +6674,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="179" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>372</v>
       </c>
@@ -6696,7 +6695,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="180" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>372</v>
       </c>
@@ -6717,7 +6716,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>375</v>
       </c>
@@ -6738,7 +6737,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>377</v>
       </c>
@@ -6759,7 +6758,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="183" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>379</v>
       </c>
@@ -6780,7 +6779,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="184" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>382</v>
       </c>
@@ -6801,7 +6800,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="185" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>384</v>
       </c>
@@ -6822,7 +6821,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="186" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>384</v>
       </c>
@@ -6843,7 +6842,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="187" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>387</v>
       </c>
@@ -6864,7 +6863,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="188" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>389</v>
       </c>
@@ -6885,7 +6884,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="189" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>391</v>
       </c>
@@ -6906,7 +6905,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="190" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>393</v>
       </c>
@@ -6927,7 +6926,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="191" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>396</v>
       </c>
@@ -6948,7 +6947,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="192" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>398</v>
       </c>
@@ -6969,7 +6968,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="193" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>402</v>
       </c>
@@ -6990,7 +6989,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="194" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>406</v>
       </c>
@@ -7011,7 +7010,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="195" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>408</v>
       </c>
@@ -7032,7 +7031,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="196" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>826</v>
       </c>
@@ -7053,7 +7052,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="197" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>411</v>
       </c>
@@ -7074,7 +7073,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="198" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>411</v>
       </c>
@@ -7095,7 +7094,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="199" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>411</v>
       </c>
@@ -7116,7 +7115,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="200" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>415</v>
       </c>
@@ -7137,7 +7136,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="201" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>415</v>
       </c>
@@ -7158,7 +7157,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="202" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>418</v>
       </c>
@@ -7179,7 +7178,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="203" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>421</v>
       </c>
@@ -7200,7 +7199,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="204" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>424</v>
       </c>
@@ -7221,7 +7220,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="205" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>424</v>
       </c>
@@ -7242,7 +7241,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="206" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>428</v>
       </c>
@@ -7263,7 +7262,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="207" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>428</v>
       </c>
@@ -7284,7 +7283,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="208" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>431</v>
       </c>
@@ -7305,7 +7304,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="209" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>434</v>
       </c>
@@ -7326,7 +7325,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="210" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>436</v>
       </c>
@@ -7347,7 +7346,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="211" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>438</v>
       </c>
@@ -7368,7 +7367,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="212" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>440</v>
       </c>
@@ -7389,7 +7388,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="213" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>442</v>
       </c>
@@ -7410,7 +7409,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="214" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>445</v>
       </c>
@@ -7431,7 +7430,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="215" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>447</v>
       </c>
@@ -7452,7 +7451,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="216" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>447</v>
       </c>
@@ -7473,7 +7472,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="217" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>447</v>
       </c>
@@ -7494,7 +7493,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="218" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>808</v>
       </c>
@@ -7515,7 +7514,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="219" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>453</v>
       </c>
@@ -7536,7 +7535,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="220" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>455</v>
       </c>
@@ -7557,7 +7556,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="221" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>457</v>
       </c>
@@ -7620,7 +7619,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="224" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>464</v>
       </c>
@@ -7641,7 +7640,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="225" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>466</v>
       </c>
@@ -7662,7 +7661,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="226" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>468</v>
       </c>
@@ -7683,7 +7682,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="227" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>470</v>
       </c>
@@ -7704,7 +7703,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="228" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>473</v>
       </c>
@@ -7725,7 +7724,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="229" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>475</v>
       </c>
@@ -7746,7 +7745,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="230" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>478</v>
       </c>
@@ -7767,7 +7766,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="231" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>480</v>
       </c>
@@ -7788,7 +7787,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="232" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>482</v>
       </c>
@@ -7809,7 +7808,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="233" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>484</v>
       </c>
@@ -7830,7 +7829,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="234" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>486</v>
       </c>
@@ -7851,7 +7850,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="235" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>489</v>
       </c>
@@ -7872,7 +7871,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="236" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>491</v>
       </c>
@@ -7893,7 +7892,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="237" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>493</v>
       </c>
@@ -7935,7 +7934,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="239" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>497</v>
       </c>
@@ -7956,7 +7955,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="240" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>499</v>
       </c>
@@ -7977,7 +7976,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="241" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>502</v>
       </c>
@@ -7998,7 +7997,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="242" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>505</v>
       </c>
@@ -8019,7 +8018,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="243" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>507</v>
       </c>
@@ -8040,7 +8039,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="244" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>509</v>
       </c>
@@ -8061,7 +8060,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="245" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>511</v>
       </c>
@@ -8082,7 +8081,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="246" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>514</v>
       </c>
@@ -8103,7 +8102,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="247" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>516</v>
       </c>
@@ -8124,7 +8123,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="248" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>828</v>
       </c>
@@ -8145,7 +8144,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="249" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>519</v>
       </c>
@@ -8166,7 +8165,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="250" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>522</v>
       </c>
@@ -8187,7 +8186,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="251" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>524</v>
       </c>
@@ -8208,7 +8207,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="252" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>526</v>
       </c>
@@ -8229,7 +8228,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="253" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>528</v>
       </c>
@@ -8250,7 +8249,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="254" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>530</v>
       </c>
@@ -8271,7 +8270,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="255" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>533</v>
       </c>
@@ -8292,7 +8291,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="256" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>535</v>
       </c>
@@ -8313,7 +8312,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="257" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>537</v>
       </c>
@@ -8355,7 +8354,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="259" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>541</v>
       </c>
@@ -8376,7 +8375,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="260" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>543</v>
       </c>
@@ -8397,7 +8396,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="261" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>829</v>
       </c>
@@ -8418,7 +8417,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="262" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>546</v>
       </c>
@@ -8439,7 +8438,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="263" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>548</v>
       </c>
@@ -8460,7 +8459,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="264" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>551</v>
       </c>
@@ -8481,7 +8480,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="265" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>553</v>
       </c>
@@ -8502,7 +8501,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="266" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>555</v>
       </c>
@@ -8523,7 +8522,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="267" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>557</v>
       </c>
@@ -8544,7 +8543,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="268" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>557</v>
       </c>
@@ -8565,7 +8564,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="269" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>560</v>
       </c>
@@ -8586,7 +8585,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="270" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>562</v>
       </c>
@@ -8607,7 +8606,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="271" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>564</v>
       </c>
@@ -8628,7 +8627,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="272" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>566</v>
       </c>
@@ -8649,7 +8648,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="273" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>568</v>
       </c>
@@ -8670,7 +8669,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="274" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>570</v>
       </c>
@@ -8691,7 +8690,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="275" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>572</v>
       </c>
@@ -8712,7 +8711,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="276" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>574</v>
       </c>
@@ -8733,7 +8732,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="277" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>574</v>
       </c>
@@ -8754,7 +8753,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="278" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>577</v>
       </c>
@@ -8775,7 +8774,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="279" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>577</v>
       </c>
@@ -8796,7 +8795,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="280" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>580</v>
       </c>
@@ -8817,7 +8816,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="281" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>582</v>
       </c>
@@ -8838,7 +8837,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="282" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>584</v>
       </c>
@@ -8859,7 +8858,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="283" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>586</v>
       </c>
@@ -8880,7 +8879,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="284" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>588</v>
       </c>
@@ -8901,7 +8900,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="285" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>590</v>
       </c>
@@ -8922,7 +8921,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="286" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>592</v>
       </c>
@@ -8943,7 +8942,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="287" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>595</v>
       </c>
@@ -8964,7 +8963,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="288" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>597</v>
       </c>
@@ -8985,7 +8984,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="289" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>597</v>
       </c>
@@ -9006,7 +9005,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="290" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>600</v>
       </c>
@@ -9027,7 +9026,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="291" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>603</v>
       </c>
@@ -9048,7 +9047,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="292" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>605</v>
       </c>
@@ -9069,7 +9068,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="293" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>608</v>
       </c>
@@ -9090,7 +9089,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="294" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>610</v>
       </c>
@@ -9111,7 +9110,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="295" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>612</v>
       </c>
@@ -9132,7 +9131,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="296" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>614</v>
       </c>
@@ -9153,7 +9152,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="297" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>616</v>
       </c>
@@ -9174,7 +9173,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="298" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>616</v>
       </c>
@@ -9195,7 +9194,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="299" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>619</v>
       </c>
@@ -9216,7 +9215,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="300" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>621</v>
       </c>
@@ -9237,7 +9236,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="301" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>623</v>
       </c>
@@ -9258,7 +9257,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="302" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>626</v>
       </c>
@@ -9279,7 +9278,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="303" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>628</v>
       </c>
@@ -9300,7 +9299,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="304" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>631</v>
       </c>
@@ -9321,7 +9320,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="305" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>631</v>
       </c>
@@ -9342,7 +9341,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="306" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>634</v>
       </c>
@@ -9363,7 +9362,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="307" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>634</v>
       </c>
@@ -9384,7 +9383,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="308" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>637</v>
       </c>
@@ -9405,7 +9404,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="309" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>639</v>
       </c>
@@ -9426,7 +9425,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="310" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>641</v>
       </c>
@@ -9468,7 +9467,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="312" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>645</v>
       </c>
@@ -9552,7 +9551,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="316" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>651</v>
       </c>
@@ -9573,7 +9572,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="317" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>653</v>
       </c>
@@ -9594,7 +9593,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="318" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>653</v>
       </c>
@@ -9615,7 +9614,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="319" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>653</v>
       </c>
@@ -9636,7 +9635,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="320" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>657</v>
       </c>
@@ -9657,7 +9656,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="321" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>830</v>
       </c>
@@ -9678,7 +9677,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="322" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>660</v>
       </c>
@@ -9699,7 +9698,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="323" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>662</v>
       </c>
@@ -9720,7 +9719,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="324" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>664</v>
       </c>
@@ -9741,7 +9740,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="325" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>664</v>
       </c>
@@ -9762,7 +9761,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="326" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>664</v>
       </c>
@@ -9783,7 +9782,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="327" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>668</v>
       </c>
@@ -9804,7 +9803,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="328" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>668</v>
       </c>
@@ -9825,7 +9824,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="329" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>668</v>
       </c>
@@ -9846,7 +9845,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="330" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>672</v>
       </c>
@@ -9867,7 +9866,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="331" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>674</v>
       </c>
@@ -9888,7 +9887,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="332" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>676</v>
       </c>
@@ -9909,7 +9908,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="333" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>678</v>
       </c>
@@ -9930,7 +9929,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="334" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>680</v>
       </c>
@@ -9951,7 +9950,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="335" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>809</v>
       </c>
@@ -9972,7 +9971,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="336" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>683</v>
       </c>
@@ -9993,7 +9992,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="337" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>686</v>
       </c>
@@ -10014,7 +10013,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="338" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>689</v>
       </c>
@@ -10035,7 +10034,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="339" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>691</v>
       </c>
@@ -10056,7 +10055,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="340" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>831</v>
       </c>
@@ -10077,7 +10076,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="341" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>831</v>
       </c>
@@ -10098,7 +10097,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="342" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>695</v>
       </c>
@@ -10119,7 +10118,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="343" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>698</v>
       </c>
@@ -10140,7 +10139,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="344" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>700</v>
       </c>
@@ -10161,7 +10160,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="345" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>700</v>
       </c>
@@ -10182,7 +10181,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="346" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>704</v>
       </c>
@@ -10203,7 +10202,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="347" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>832</v>
       </c>
@@ -10224,7 +10223,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="348" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>833</v>
       </c>
@@ -10245,7 +10244,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="349" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>708</v>
       </c>
@@ -10266,7 +10265,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="350" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>710</v>
       </c>
@@ -10287,7 +10286,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="351" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>712</v>
       </c>
@@ -10371,7 +10370,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="355" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>718</v>
       </c>
@@ -10392,7 +10391,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="356" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>718</v>
       </c>
@@ -10413,7 +10412,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="357" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>722</v>
       </c>
@@ -10434,7 +10433,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="358" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>724</v>
       </c>
@@ -10455,7 +10454,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="359" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>834</v>
       </c>
@@ -10476,7 +10475,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="360" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>727</v>
       </c>
@@ -10497,7 +10496,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="361" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>727</v>
       </c>
@@ -10518,7 +10517,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="362" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>730</v>
       </c>
@@ -10539,7 +10538,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="363" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>732</v>
       </c>
@@ -10560,7 +10559,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="364" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>735</v>
       </c>
@@ -10581,7 +10580,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="365" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>737</v>
       </c>
@@ -10602,7 +10601,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="366" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>739</v>
       </c>
@@ -10623,7 +10622,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="367" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>741</v>
       </c>
@@ -10644,7 +10643,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="368" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>743</v>
       </c>
@@ -10665,7 +10664,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="369" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>745</v>
       </c>
@@ -10728,7 +10727,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="372" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>749</v>
       </c>
@@ -10749,7 +10748,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="373" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>751</v>
       </c>
@@ -10770,7 +10769,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="374" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>753</v>
       </c>
@@ -10791,7 +10790,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="375" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>755</v>
       </c>
@@ -10812,7 +10811,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="376" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>757</v>
       </c>
@@ -10833,7 +10832,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="377" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>759</v>
       </c>
@@ -10854,7 +10853,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="378" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>759</v>
       </c>
@@ -10875,7 +10874,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="379" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>759</v>
       </c>
@@ -10896,7 +10895,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="380" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>763</v>
       </c>
@@ -10917,7 +10916,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="381" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>763</v>
       </c>
@@ -10938,7 +10937,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="382" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>766</v>
       </c>
@@ -10959,7 +10958,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="383" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>768</v>
       </c>
@@ -10980,7 +10979,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="384" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>770</v>
       </c>
@@ -11001,7 +11000,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="385" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>836</v>
       </c>
@@ -11022,7 +11021,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="386" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>773</v>
       </c>
@@ -11043,7 +11042,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="387" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>775</v>
       </c>
@@ -11064,7 +11063,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="388" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>777</v>
       </c>
@@ -11085,7 +11084,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="389" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>779</v>
       </c>
@@ -11106,7 +11105,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="390" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>781</v>
       </c>
@@ -11127,7 +11126,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="391" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>783</v>
       </c>
@@ -11148,7 +11147,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="392" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>785</v>
       </c>
@@ -11169,7 +11168,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="393" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>787</v>
       </c>
@@ -11190,7 +11189,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="394" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>789</v>
       </c>
@@ -11211,7 +11210,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="395" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>791</v>
       </c>
@@ -11232,7 +11231,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="396" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>793</v>
       </c>
@@ -11253,7 +11252,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="397" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>793</v>
       </c>
@@ -11274,7 +11273,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="398" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>796</v>
       </c>
@@ -11295,7 +11294,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="399" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>799</v>
       </c>
@@ -11316,7 +11315,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="400" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>801</v>
       </c>
@@ -11337,7 +11336,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="401" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>803</v>
       </c>
@@ -11359,13 +11358,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F401" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="Energia Elétrica"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:F401" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>